<commit_message>
Added an entry (prototype UI)
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shane\Documents\College\Fall 2018\POO SD\Testy\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8E98CE04-2504-4DF3-987C-8154A4B1A766}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AB7703E3-E4A4-4430-9021-8BB34C4008A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="10140" xr2:uid="{CA794E77-CD3F-4E74-B305-22302D3F0C68}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>If the app is deleted or the phone is factory reset, the data and profile does not dissappear.</t>
+  </si>
+  <si>
+    <t>As a developer, I want to create a prototype of the UI.</t>
+  </si>
+  <si>
+    <t>The prototype is created to make it easier to implement in Android Studio.</t>
   </si>
 </sst>
 </file>
@@ -188,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -211,6 +217,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -218,7 +266,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -234,6 +282,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -554,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC01BA41-E1D9-4073-B602-F537DFF1B952}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,27 +815,35 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="9">
         <v>2</v>
       </c>
       <c r="C15" s="4">
         <v>5</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="11">
+        <v>1</v>
+      </c>
+      <c r="C16" s="11">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -791,7 +857,7 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>